<commit_message>
part# analysis;reconcile app and pdic forecast
</commit_message>
<xml_diff>
--- a/pidsg25-06.xlsx
+++ b/pidsg25-06.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/debdeeppaul/Documents/Procurement/PIDSG25/forecast25/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26F237BD-C81D-1B49-A2C8-BF9B759C924B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4D861AC-504B-E84C-BBB4-BBAA39C52A36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3340" yWindow="500" windowWidth="17100" windowHeight="10960" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3340" yWindow="500" windowWidth="21100" windowHeight="11860" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="from_alvin" sheetId="1" r:id="rId1"/>
@@ -285,10 +285,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -3461,15 +3461,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>31750</xdr:colOff>
-      <xdr:row>56</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:colOff>387350</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>488950</xdr:colOff>
-      <xdr:row>70</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:colOff>844550</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3686,10 +3686,10 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B3" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="10"/>
+      <c r="B3" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="11"/>
       <c r="D3" s="1">
         <v>45383</v>
       </c>
@@ -4151,10 +4151,10 @@
       </c>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="10"/>
+      <c r="C14" s="11"/>
       <c r="D14" s="1">
         <v>45748</v>
       </c>
@@ -6185,8 +6185,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39C0A8C1-78FE-4A69-B39B-104D697149B8}">
   <dimension ref="B3:M69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I60" sqref="I60"/>
+    <sheetView tabSelected="1" topLeftCell="A47" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J59" sqref="J59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7657,7 +7657,7 @@
       <c r="F60" s="7">
         <v>45833</v>
       </c>
-      <c r="G60" s="11">
+      <c r="G60" s="10">
         <v>185342.5</v>
       </c>
       <c r="H60">
@@ -7672,7 +7672,7 @@
       <c r="F61" s="7">
         <v>45863</v>
       </c>
-      <c r="G61" s="11">
+      <c r="G61" s="10">
         <v>211816.5</v>
       </c>
       <c r="H61">
@@ -7687,7 +7687,7 @@
       <c r="F62" s="7">
         <v>45894</v>
       </c>
-      <c r="G62" s="11">
+      <c r="G62" s="10">
         <v>208414.5</v>
       </c>
       <c r="H62">
@@ -7702,7 +7702,7 @@
       <c r="F63" s="7">
         <v>45925</v>
       </c>
-      <c r="G63" s="11">
+      <c r="G63" s="10">
         <v>204928.5</v>
       </c>
       <c r="H63">
@@ -7717,7 +7717,7 @@
       <c r="F64" s="7">
         <v>45955</v>
       </c>
-      <c r="G64" s="11">
+      <c r="G64" s="10">
         <v>201565</v>
       </c>
       <c r="H64">
@@ -7732,7 +7732,7 @@
       <c r="F65" s="7">
         <v>45986</v>
       </c>
-      <c r="G65" s="11">
+      <c r="G65" s="10">
         <v>198121</v>
       </c>
       <c r="H65">
@@ -7747,7 +7747,7 @@
       <c r="F66" s="7">
         <v>46016</v>
       </c>
-      <c r="G66" s="11">
+      <c r="G66" s="10">
         <v>155050</v>
       </c>
       <c r="H66">
@@ -7762,7 +7762,7 @@
       <c r="F67" s="7">
         <v>46047</v>
       </c>
-      <c r="G67" s="11">
+      <c r="G67" s="10">
         <v>154700</v>
       </c>
       <c r="H67">
@@ -7777,7 +7777,7 @@
       <c r="F68" s="7">
         <v>46078</v>
       </c>
-      <c r="G68" s="11">
+      <c r="G68" s="10">
         <v>133350</v>
       </c>
       <c r="H68">
@@ -7792,7 +7792,7 @@
       <c r="F69" s="7">
         <v>46106</v>
       </c>
-      <c r="G69" s="11">
+      <c r="G69" s="10">
         <v>132650</v>
       </c>
       <c r="H69">

</xml_diff>